<commit_message>
fixed to unit 05 - spelling mistake and image, previuos exam names and year
</commit_message>
<xml_diff>
--- a/tamil_biology/unit_05_plant_physiology.xlsx
+++ b/tamil_biology/unit_05_plant_physiology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2020\git\tvmani.github.io\tamil_biology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17657EF-388A-4AAF-850D-D8ED5481C829}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4742FB65-77F8-4B9A-859A-5B5E95255787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="334">
   <si>
     <t>question_no</t>
   </si>
@@ -789,9 +789,6 @@
     <t>தக்காளியானது ஒரு பசுமை இல்ல தாவரமாகும் CO2 செறிவு அதிகமான இடங்களில் விளைச்சல் அதிகரிக்கும்.</t>
   </si>
   <si>
-    <t>உனது தோட்டத்தில் வளரும் ஒரு தாவராமானது ஒளிசுவாச இழப்பினை தவிர்க்கிறது. நீரை பயன்படுத்தும் திறன், அதிக வெப்பத்தில் அதிக ஒளிசேர்க்கை வீதம் மற்றும் அதிக நைட்ரஜன் பயன்படுத்தும் திறன் பெற்றுள்ள இத்தாவரத்தினை கண்டறிக.</t>
-  </si>
-  <si>
     <t>NEET Phase</t>
   </si>
   <si>
@@ -855,9 +852,6 @@
     <t xml:space="preserve">ATP யில் பாஸ்பேட் தொகுதி சேர்க்கப்படுதல் </t>
   </si>
   <si>
-    <t xml:space="preserve">தளப்பொருள் ஆக்ஸிஜனேற்றத்தின் போது எலக்ட்ரான்களில் வெளியேரும் ஆற்றலைப் பயன்படுத்தி ATP உருவாகிறது. </t>
-  </si>
-  <si>
     <t>கொழுப்பு, கார்போஹைட்ரேட்கள் மற்றும் புரதங்களின் சுவாசித்தல் வழி உடைதலுக்கு எந்த உயிரி மூலக்கூறு பொதுவானது?</t>
   </si>
   <si>
@@ -879,21 +873,9 @@
     <t xml:space="preserve">அசிட்டைல்CoA </t>
   </si>
   <si>
-    <t>கிரப்ஸ் சுழற்சியைபொருத்தவரை எது தவறான கூற்று?</t>
-  </si>
-  <si>
     <t xml:space="preserve">இந்த சுழற்சியில் ஒரு புள்ளியில் FAD வானது FADH2வாக ஒடுக்கமடைகிறது </t>
   </si>
   <si>
-    <t xml:space="preserve">சக்சினைல் CoA சக்சினிக் அமிலமாக மாறும்போது GTP என்ற மூலக்கூறு உருவாகிறது </t>
-  </si>
-  <si>
-    <t xml:space="preserve">இந்தசுழற்சியில் அசிட்டைல் தொகுதியுடன் (அசிட்டைல் CoA) பைருவிக் அமிலத்துடன் இணைந்து சிட்ரிக்அமிலம் உருவாகிறது </t>
-  </si>
-  <si>
-    <t xml:space="preserve">இந்த சுழற்சியில் மூன்று இடங்கள் NAD+னது NADH+ H+க ஒடுக்கமடைகிறது. </t>
-  </si>
-  <si>
     <t xml:space="preserve">வளர்சிதை மாற்றத்தின் போது தளப்பொருள் ஆக்ஸிஜனேற்றத்தின் வெளியேறும் ஆற்றலை எலக்ட்ரான் ஏற்கும் நிகழ்விற்கு பெயர் </t>
   </si>
   <si>
@@ -918,15 +900,6 @@
     <t xml:space="preserve">மாலிக்அமிலம் , அசிட்டைல் இணைநொதி </t>
   </si>
   <si>
-    <t xml:space="preserve">ஆக்சலோ அசிட்டிக் அமிலம் , அசிட்டைல் இணைநொதி </t>
-  </si>
-  <si>
-    <t xml:space="preserve">சக்சினிக் அமிலம் , பைருவிக் அமிலம் </t>
-  </si>
-  <si>
-    <t>பியுமாரிக்அமிலம் , பைருவிக் அமிலம்</t>
-  </si>
-  <si>
     <t xml:space="preserve">சுவாசித்தல் என்ற வினையில் </t>
   </si>
   <si>
@@ -1029,9 +1002,6 @@
     <t>உடலமுறை உற்பத்தி வாழைக்கனி</t>
   </si>
   <si>
-    <t>ஆக்சீன் தெளித்தல்</t>
-  </si>
-  <si>
     <t xml:space="preserve">அ மற்றும் ஆ </t>
   </si>
   <si>
@@ -1047,18 +1017,12 @@
     <t xml:space="preserve">IAA </t>
   </si>
   <si>
-    <t xml:space="preserve">அவினா வளைவுச் சோதனை எனும் உயிரிய ஆய்வு இதன் செயல்பட்டினை அறிய உதவுகிறது </t>
-  </si>
-  <si>
     <t>AIIMS, NEET</t>
   </si>
   <si>
     <t>2006, 2016</t>
   </si>
   <si>
-    <t>செயற்கை ஆக்சீன் என்பது எது ?</t>
-  </si>
-  <si>
     <t xml:space="preserve">IBA </t>
   </si>
   <si>
@@ -1101,18 +1065,12 @@
     <t xml:space="preserve">தக்காளி </t>
   </si>
   <si>
-    <t xml:space="preserve">தேயிலை பயிரிடும்போது பயன்படுத்தப்படும் </t>
-  </si>
-  <si>
     <t xml:space="preserve">சியாடின் </t>
   </si>
   <si>
     <t xml:space="preserve">வேர் வளர்ச்சியை தூண்டுவது </t>
   </si>
   <si>
-    <t xml:space="preserve">ஆக்சீன் </t>
-  </si>
-  <si>
     <t>ஜிப்ரலின்</t>
   </si>
   <si>
@@ -1131,9 +1089,6 @@
     <t>இலை உதிர்தல்</t>
   </si>
   <si>
-    <t xml:space="preserve">ஓர் செயற்கையான வளர்ப்பு முறையில் வேறுபாடு அடையச் செய்வதற்கு உங்களிடம் திசு கொடுக்கப்படுகிறது கீழ்க்கண்ட எந்த இரண்டு ஹார்மோன்களை வளர்ப்பு ஊடகத்தில் நீங்கள் சேர்ப்பதால் திசுவிலிருந்து வேறு மற்றும் தண்டுத்தொகுப்பில் உருவாக்கப்படுகிறது. </t>
-  </si>
-  <si>
     <t xml:space="preserve">ஜிப்ரலின்கள் மற்றும் அப்சசிக் அமிலம் </t>
   </si>
   <si>
@@ -1177,13 +1132,110 @@
   </si>
   <si>
     <t>செல்லின் உட்புறத்தே காணப்படுகின்ற கரைசல்?</t>
+  </si>
+  <si>
+    <t>உனது தோட்டத்தில் வளரும் ஒரு தாவரமானது ஒளிசுவாச இழப்பினை தவிர்க்கிறது. நீரை பயன்படுத்தும் திறன், அதிக வெப்பத்தில் அதிக ஒளிசேர்க்கை வீதம் மற்றும் அதிக நைட்ரஜன் பயன்படுத்தும் திறன் பெற்றுள்ள இத்தாவரத்தினை கண்டறிக.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">தளப்பொருள் ஆக்ஸிஜனேற்றத்தின் போது எலக்ட்ரான்களில் வெளியேறும் ஆற்றலைப் பயன்படுத்தி ATP உருவாகிறது. </t>
+  </si>
+  <si>
+    <t>கிரப்ஸ் சுழற்சியை பொருத்தவரை எது தவறான கூற்று?</t>
+  </si>
+  <si>
+    <t>சக்சினைல் CoA சக்சினிக் அமிலமாக மாறும்போது GTP என்ற மூலக்கூறு உருவாகிறது</t>
+  </si>
+  <si>
+    <t xml:space="preserve">இந்த சுழற்சியில் அசிட்டைல் தொகுதியுடன் (அசிட்டைல் CoA) பைருவிக் அமிலத்துடன் இணைந்து சிட்ரிக் அமிலம் உருவாகிறது </t>
+  </si>
+  <si>
+    <t xml:space="preserve">இந்த சுழற்சியில் மூன்று இடங்களில் NAD+ ஆனது NADH+ H+ ஆக ஒடுக்கமடைகிறது. </t>
+  </si>
+  <si>
+    <t>ATP</t>
+  </si>
+  <si>
+    <r>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FAD (அல்லது) FADH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>NADH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ஆக்சலோ அசிட்டிக் அமிலம், அசிட்டைல் இணைநொதி </t>
+  </si>
+  <si>
+    <t xml:space="preserve">சக்சினிக் அமிலம், பைருவிக் அமிலம் </t>
+  </si>
+  <si>
+    <t>பியுமாரிக்அமிலம், பைருவிக் அமிலம்</t>
+  </si>
+  <si>
+    <t>ஆக்சின் தெளித்தல்</t>
+  </si>
+  <si>
+    <t xml:space="preserve">அவினா வளைவுச் சோதனை எனும் உயிரியல் ஆய்வு இதன் செயல்பாட்டினை அறிய உதவுகிறது </t>
+  </si>
+  <si>
+    <t>செயற்கை ஆக்சின் என்பது எது ?</t>
+  </si>
+  <si>
+    <t>தேயிலை பயிரிடும்போது எது பயன்படுத்தப்படும்?</t>
+  </si>
+  <si>
+    <t>ஓர் செயற்கையான வளர்ப்பு முறையில் வேறுபாடு அடையச் செய்வதற்கு உங்களிடம் திசு கொடுக்கப்படுகிறது. கீழ்க்கண்ட எந்த இரண்டு ஹார்மோன்களை வளர்ப்பு ஊடகத்தில் நீங்கள் சேர்ப்பதால் திசுவிலிருந்து வேர் மற்றும் தண்டுத்தொகுப்பில் உருவாக்கப்படுகிறது?</t>
+  </si>
+  <si>
+    <t>காற்று  சுவாசித்தலின்போது இந்த வரைபடத்தில்
+உள்ள பெட்டியானது மூன்று முக்கிய
+உயிரிவழித்தடத்தினை குறிக்கிறது மற்றும்
+அம்புக்குறி நிகரவினை அல்லது விளைபொருளை
+குறிக்கிறது.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1219,6 +1271,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1240,7 +1300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1261,6 +1321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1303,7 +1364,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I63" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I64" totalsRowShown="0" headerRowDxfId="0">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="question_no"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="question"/>
@@ -1640,15 +1701,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" customWidth="1"/>
     <col min="2" max="2" width="61.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="22.109375" customWidth="1"/>
@@ -2097,7 +2158,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="C16" t="s">
         <v>89</v>
@@ -2700,10 +2761,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C37" t="s">
         <v>200</v>
-      </c>
-      <c r="C37" t="s">
-        <v>201</v>
       </c>
       <c r="D37">
         <v>2016</v>
@@ -2712,13 +2773,13 @@
         <v>192</v>
       </c>
       <c r="F37" t="s">
+        <v>201</v>
+      </c>
+      <c r="G37" t="s">
         <v>202</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>203</v>
-      </c>
-      <c r="H37" t="s">
-        <v>204</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -2729,25 +2790,25 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D38">
         <v>2016</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>163</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I38">
         <v>1</v>
@@ -2758,25 +2819,25 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C39" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D39">
         <v>2016</v>
       </c>
       <c r="E39" t="s">
+        <v>209</v>
+      </c>
+      <c r="F39" t="s">
         <v>210</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>211</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>212</v>
-      </c>
-      <c r="H39" t="s">
-        <v>213</v>
       </c>
       <c r="I39">
         <v>3</v>
@@ -2787,22 +2848,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D40">
         <v>2016</v>
       </c>
       <c r="E40" t="s">
+        <v>214</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" t="s">
         <v>216</v>
-      </c>
-      <c r="G40" t="s">
-        <v>217</v>
       </c>
       <c r="H40" t="s">
         <v>166</v>
@@ -2816,7 +2877,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
@@ -2825,16 +2886,16 @@
         <v>2016</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="H41" s="2" t="s">
-        <v>222</v>
+        <v>316</v>
       </c>
       <c r="I41">
         <v>4</v>
@@ -2845,36 +2906,36 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C42" t="s">
+        <v>222</v>
+      </c>
+      <c r="D42" t="s">
         <v>223</v>
       </c>
-      <c r="C42" t="s">
+      <c r="E42" t="s">
         <v>224</v>
       </c>
-      <c r="D42" t="s">
+      <c r="F42" t="s">
         <v>225</v>
       </c>
-      <c r="E42" t="s">
+      <c r="G42" t="s">
         <v>226</v>
       </c>
-      <c r="F42" t="s">
+      <c r="H42" t="s">
         <v>227</v>
-      </c>
-      <c r="G42" t="s">
-        <v>228</v>
-      </c>
-      <c r="H42" t="s">
-        <v>229</v>
       </c>
       <c r="I42">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>230</v>
+        <v>317</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
@@ -2883,433 +2944,433 @@
         <v>2017</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>232</v>
+        <v>318</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>233</v>
+        <v>319</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>234</v>
+        <v>320</v>
       </c>
       <c r="I43">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="72.599999999999994" x14ac:dyDescent="0.35">
       <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>2013</v>
+      </c>
+      <c r="E44" t="s">
+        <v>321</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="G44" t="s">
+        <v>323</v>
+      </c>
+      <c r="H44" t="s">
+        <v>324</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C45" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45">
+        <v>2010</v>
+      </c>
+      <c r="E45" t="s">
+        <v>230</v>
+      </c>
+      <c r="F45" t="s">
+        <v>231</v>
+      </c>
+      <c r="G45" t="s">
+        <v>232</v>
+      </c>
+      <c r="H45" t="s">
+        <v>233</v>
+      </c>
+      <c r="I45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="8">
+        <v>45</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C46" t="s">
         <v>235</v>
-      </c>
-      <c r="C44" t="s">
-        <v>140</v>
-      </c>
-      <c r="D44">
-        <v>2010</v>
-      </c>
-      <c r="E44" t="s">
-        <v>236</v>
-      </c>
-      <c r="F44" t="s">
-        <v>237</v>
-      </c>
-      <c r="G44" t="s">
-        <v>238</v>
-      </c>
-      <c r="H44" t="s">
-        <v>239</v>
-      </c>
-      <c r="I44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A45" s="8">
-        <v>45</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="C45" t="s">
-        <v>241</v>
-      </c>
-      <c r="D45">
-        <v>1980</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="I45" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="8">
-        <v>46</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="C46" t="s">
-        <v>241</v>
       </c>
       <c r="D46">
         <v>1980</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>248</v>
+        <v>325</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>249</v>
+        <v>326</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>250</v>
+        <v>327</v>
       </c>
       <c r="I46" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="8">
+        <v>46</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="C47" t="s">
+        <v>235</v>
+      </c>
+      <c r="D47">
+        <v>1980</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="I47" s="9">
         <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="8">
-        <v>47</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="C47" t="s">
-        <v>241</v>
-      </c>
-      <c r="D47">
-        <v>1984</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="I47" s="9">
-        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
-        <v>48</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>256</v>
+        <v>47</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>242</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>235</v>
       </c>
       <c r="D48">
         <v>1984</v>
       </c>
-      <c r="E48" s="8" t="s">
-        <v>257</v>
+      <c r="E48" s="9" t="s">
+        <v>243</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>259</v>
+        <v>244</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>245</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="I48" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
-        <v>49</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>261</v>
+        <v>48</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>247</v>
       </c>
       <c r="C49" t="s">
         <v>101</v>
       </c>
       <c r="D49">
-        <v>1989</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>262</v>
+        <v>1984</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>248</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="I49" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
+        <v>49</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C50" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50">
+        <v>1989</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="I50" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="8">
         <v>50</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="C50" t="s">
-        <v>267</v>
-      </c>
-      <c r="D50">
+      <c r="B51" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C51" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51">
         <v>2000</v>
       </c>
-      <c r="E50" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="I50" s="9">
+      <c r="E51" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="I51" s="9">
         <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="8">
-        <v>51</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="C51" t="s">
-        <v>273</v>
-      </c>
-      <c r="D51">
-        <v>2003</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="I51" s="9">
-        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
+        <v>51</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C52" t="s">
+        <v>264</v>
+      </c>
+      <c r="D52">
+        <v>2003</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="I52" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="8">
         <v>52</v>
       </c>
-      <c r="B52" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B53" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C53" t="s">
         <v>45</v>
-      </c>
-      <c r="D52">
-        <v>2004</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="I52" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="8">
-        <v>53</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="C53" t="s">
-        <v>101</v>
       </c>
       <c r="D53">
         <v>2004</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="H53" s="9" t="s">
-        <v>277</v>
+        <v>270</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>272</v>
       </c>
       <c r="I53" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
+        <v>53</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C54" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54">
+        <v>2004</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="I54" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="8">
         <v>54</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B55" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="C55" t="s">
+        <v>276</v>
+      </c>
+      <c r="D55" t="s">
+        <v>277</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="I55" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="8">
+        <v>55</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C56" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56">
+        <v>2004</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I56" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="8">
+        <v>56</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C57" t="s">
+        <v>282</v>
+      </c>
+      <c r="D57">
+        <v>2009</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="H57" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="C54" t="s">
+      <c r="I57" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="8">
+        <v>57</v>
+      </c>
+      <c r="B58" s="9" t="s">
         <v>287</v>
-      </c>
-      <c r="D54" t="s">
-        <v>288</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="I54" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="8">
-        <v>55</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="C55" t="s">
-        <v>140</v>
-      </c>
-      <c r="D55">
-        <v>2004</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="G55" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="H55" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="I55" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="8">
-        <v>56</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="C56" t="s">
-        <v>294</v>
-      </c>
-      <c r="D56">
-        <v>2009</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="H56" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="I56" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="8">
-        <v>57</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="C57" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57">
-        <v>2010</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="G57" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="H57" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="I57" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="8">
-        <v>58</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>304</v>
       </c>
       <c r="C58" t="s">
         <v>140</v>
@@ -3317,28 +3378,28 @@
       <c r="D58">
         <v>2010</v>
       </c>
-      <c r="E58" s="8" t="s">
-        <v>276</v>
+      <c r="E58" s="9" t="s">
+        <v>288</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="G58" s="9" t="s">
-        <v>297</v>
+        <v>289</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>290</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="I58" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>306</v>
+        <v>331</v>
       </c>
       <c r="C59" t="s">
         <v>140</v>
@@ -3346,86 +3407,86 @@
       <c r="D59">
         <v>2010</v>
       </c>
-      <c r="E59" s="9" t="s">
-        <v>307</v>
+      <c r="E59" s="8" t="s">
+        <v>267</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="G59" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="H59" s="9" t="s">
-        <v>295</v>
+        <v>292</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="H59" s="8" t="s">
+        <v>260</v>
       </c>
       <c r="I59" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
-        <v>60</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>309</v>
+        <v>59</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>293</v>
       </c>
       <c r="C60" t="s">
         <v>140</v>
       </c>
       <c r="D60">
+        <v>2010</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="I60" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A61" s="8">
+        <v>60</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C61" t="s">
+        <v>140</v>
+      </c>
+      <c r="D61">
         <v>2008</v>
       </c>
-      <c r="E60" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="I60" s="9">
+      <c r="E61" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="I61" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="8">
+    <row r="62" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="8">
         <v>61</v>
       </c>
-      <c r="B61" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="C61" t="s">
-        <v>10</v>
-      </c>
-      <c r="D61">
-        <v>2016</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="H61" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="I61" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="8">
-        <v>62</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>319</v>
+      <c r="B62" s="9" t="s">
+        <v>332</v>
       </c>
       <c r="C62" t="s">
         <v>10</v>
@@ -3433,28 +3494,28 @@
       <c r="D62">
         <v>2016</v>
       </c>
-      <c r="E62" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="F62" s="8" t="s">
-        <v>321</v>
-      </c>
-      <c r="G62" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="H62" s="8" t="s">
-        <v>323</v>
+      <c r="E62" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>303</v>
       </c>
       <c r="I62" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="C63" t="s">
         <v>10</v>
@@ -3463,25 +3524,55 @@
         <v>2016</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>325</v>
+        <v>305</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>326</v>
+        <v>306</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>328</v>
+        <v>308</v>
       </c>
       <c r="I63" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="8">
+        <v>63</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="C64" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64">
+        <v>2016</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="I64" s="9">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
unit 05 - issues with images, sentence-semantically correct, text overlapping with footer
</commit_message>
<xml_diff>
--- a/tamil_biology/unit_05_plant_physiology.xlsx
+++ b/tamil_biology/unit_05_plant_physiology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2020\git\tvmani.github.io\tamil_biology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4742FB65-77F8-4B9A-859A-5B5E95255787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95306649-ED69-4954-B67A-AE1636897CA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -840,9 +840,6 @@
     <t xml:space="preserve">ஏற்பி கூட்டமைப்பு </t>
   </si>
   <si>
-    <t xml:space="preserve">ஆக்ஸிஜனேற்ற பாஸ்பரிகரணம் என்பது </t>
-  </si>
-  <si>
     <t xml:space="preserve">தளப்பொருளிலிருந்து பாஸ்பேட் தொகுதி ADP க்கு மாற்றப்பட்டு ATP உருவாகிறது </t>
   </si>
   <si>
@@ -900,24 +897,15 @@
     <t xml:space="preserve">மாலிக்அமிலம் , அசிட்டைல் இணைநொதி </t>
   </si>
   <si>
-    <t xml:space="preserve">சுவாசித்தல் என்ற வினையில் </t>
-  </si>
-  <si>
     <t xml:space="preserve">ஆற்றல் பயன்படுத்தப்படுகிறது </t>
   </si>
   <si>
     <t xml:space="preserve">ஆற்றல் ADP வடிவத்தில் சேமிக்கப்படுகிறது </t>
   </si>
   <si>
-    <t xml:space="preserve">ஆற்றல் TP வடிவத்தில் வெளியிடப்படுகிறது மற்றும் சேமிக்கப்படுகிறது </t>
-  </si>
-  <si>
     <t>ஆற்றல் ஒரு போதும் வெளியிடப்படுவதில்லை</t>
   </si>
   <si>
-    <t xml:space="preserve">காற்று மற்றும் காற்றிலா சுவாசித்தலில் பொதுவான நிலை எனப்படுவது </t>
-  </si>
-  <si>
     <t xml:space="preserve">கிளைக்காலைசிஸ் </t>
   </si>
   <si>
@@ -930,9 +918,6 @@
     <t xml:space="preserve">ஆக்ஸிஜனேற்ற பாஸ்பரிகரணம் </t>
   </si>
   <si>
-    <t xml:space="preserve">ATP உற்பத்திநடைபெறுகிறது </t>
-  </si>
-  <si>
     <t>உட்கூழ்மம்</t>
   </si>
   <si>
@@ -945,9 +930,6 @@
     <t xml:space="preserve">இவற்றில் எதுவுமில்லை </t>
   </si>
   <si>
-    <t xml:space="preserve">கிரப்ஸ் சுழற்சியில் உள்ள எந்த 5-கார்பன் கரிமசேர்மம் N2 வளர்சிதை மாற்றத்தில் முக்கிய சேர்மமாக உள்ளது </t>
-  </si>
-  <si>
     <t xml:space="preserve">சிட்ரிக் அமிலம் </t>
   </si>
   <si>
@@ -978,9 +960,6 @@
     <t>சியாடின்</t>
   </si>
   <si>
-    <t xml:space="preserve">இளநீரில் காணப்படும் ஹார்மோன் </t>
-  </si>
-  <si>
     <t>PMT</t>
   </si>
   <si>
@@ -996,9 +975,6 @@
     <t xml:space="preserve">சைட்டோகைனின் </t>
   </si>
   <si>
-    <t xml:space="preserve">விதையில்லா வாழைக்கனி உருவாக காரணம் </t>
-  </si>
-  <si>
     <t>உடலமுறை உற்பத்தி வாழைக்கனி</t>
   </si>
   <si>
@@ -1008,9 +984,6 @@
     <t xml:space="preserve">மேற்கூறிய எதுவுமில்லை </t>
   </si>
   <si>
-    <t xml:space="preserve">தாவர நுனிகள் துண்டிக்கப்பட்டு சீரமைக்கும் போது, கோண மொட்டின் வளர்ச்சி தூண்டப்பட்டு, கிளைகள் தோன்ற காரணமான ஹார்மோன். </t>
-  </si>
-  <si>
     <t xml:space="preserve">ஜிப்ரானிகள் </t>
   </si>
   <si>
@@ -1032,9 +1005,6 @@
     <t xml:space="preserve">GA </t>
   </si>
   <si>
-    <t xml:space="preserve">கரோட்டினாய்டு எனும் நிறமியிலிருந்து பெறப்படும் ஹார்மோன் </t>
-  </si>
-  <si>
     <t>AIIPMT</t>
   </si>
   <si>
@@ -1050,9 +1020,6 @@
     <t xml:space="preserve">ஜிப்ரலிக் அமிலம் </t>
   </si>
   <si>
-    <t xml:space="preserve">ஒளிக்காலத்துவம் முதன் முதலில் கண்டறியப்பட்ட தாவரம் </t>
-  </si>
-  <si>
     <t xml:space="preserve">பருத்தி </t>
   </si>
   <si>
@@ -1068,15 +1035,9 @@
     <t xml:space="preserve">சியாடின் </t>
   </si>
   <si>
-    <t xml:space="preserve">வேர் வளர்ச்சியை தூண்டுவது </t>
-  </si>
-  <si>
     <t>ஜிப்ரலின்</t>
   </si>
   <si>
-    <t xml:space="preserve">தாவர வளர்ச்சியில் நடைபெறும் மூப்படைதல் எனும் நிகழ்ச்சியை தெரிவிப்பது </t>
-  </si>
-  <si>
     <t xml:space="preserve">ஓராண்டுத் தாவரங்கள் </t>
   </si>
   <si>
@@ -1101,9 +1062,6 @@
     <t>ஆக்சின் மற்றும் ஜிப்ரலின்கள்</t>
   </si>
   <si>
-    <t xml:space="preserve">பைட்டோகுரோம் என்பது </t>
-  </si>
-  <si>
     <t xml:space="preserve">குரோமோபுரோட்டீன் </t>
   </si>
   <si>
@@ -1116,19 +1074,7 @@
     <t xml:space="preserve">லிப்போபுரதம் </t>
   </si>
   <si>
-    <t xml:space="preserve">தாவரங்களில் வளர்ச்சி வளைவு </t>
-  </si>
-  <si>
-    <t xml:space="preserve">நேரானது </t>
-  </si>
-  <si>
     <t xml:space="preserve">படி வடிவம் </t>
-  </si>
-  <si>
-    <t xml:space="preserve">பரவளைய </t>
-  </si>
-  <si>
-    <t xml:space="preserve">சிக்மாய்டு </t>
   </si>
   <si>
     <t>செல்லின் உட்புறத்தே காணப்படுகின்ற கரைசல்?</t>
@@ -1212,16 +1158,7 @@
     <t>ஆக்சின் தெளித்தல்</t>
   </si>
   <si>
-    <t xml:space="preserve">அவினா வளைவுச் சோதனை எனும் உயிரியல் ஆய்வு இதன் செயல்பாட்டினை அறிய உதவுகிறது </t>
-  </si>
-  <si>
-    <t>செயற்கை ஆக்சின் என்பது எது ?</t>
-  </si>
-  <si>
     <t>தேயிலை பயிரிடும்போது எது பயன்படுத்தப்படும்?</t>
-  </si>
-  <si>
-    <t>ஓர் செயற்கையான வளர்ப்பு முறையில் வேறுபாடு அடையச் செய்வதற்கு உங்களிடம் திசு கொடுக்கப்படுகிறது. கீழ்க்கண்ட எந்த இரண்டு ஹார்மோன்களை வளர்ப்பு ஊடகத்தில் நீங்கள் சேர்ப்பதால் திசுவிலிருந்து வேர் மற்றும் தண்டுத்தொகுப்பில் உருவாக்கப்படுகிறது?</t>
   </si>
   <si>
     <t>காற்று  சுவாசித்தலின்போது இந்த வரைபடத்தில்
@@ -1229,6 +1166,69 @@
 உயிரிவழித்தடத்தினை குறிக்கிறது மற்றும்
 அம்புக்குறி நிகரவினை அல்லது விளைபொருளை
 குறிக்கிறது.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ஆற்றல் ATP வடிவத்தில் வெளியிடப்படுகிறது மற்றும் சேமிக்கப்படுகிறது </t>
+  </si>
+  <si>
+    <t>சுவாசித்தல் என்ற வினையில் என்ன நிகழ்கிறது?</t>
+  </si>
+  <si>
+    <t>ஆக்ஸிஜனேற்ற பாஸ்பரிகரணம் என்பது என்ன?</t>
+  </si>
+  <si>
+    <t>ATP உற்பத்தி எங்கு நடைபெறுகிறது?</t>
+  </si>
+  <si>
+    <t>இளநீரில் காணப்படும் ஹார்மோன் எது?</t>
+  </si>
+  <si>
+    <t>விதையில்லா வாழைக்கனி உருவாக காரணம் என்ன?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">தாவர நுனிகள் துண்டிக்கப்பட்டு சீரமைக்கும் போது, கோண மொட்டின் வளர்ச்சி தூண்டப்பட்டு, கிளைகள் தோன்ற காரணமான ஹார்மோன் எது? </t>
+  </si>
+  <si>
+    <t>செயற்கை ஆக்சின் என்பது எது?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">கரோட்டினாய்டு எனும் நிறமியிலிருந்து பெறப்படும் ஹார்மோன் எது? </t>
+  </si>
+  <si>
+    <t>ஒளிக்காலத்துவம் முதன் முதலில் கண்டறியப்பட்ட தாவரத்தின் பெயர் என்ன?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">வேர் வளர்ச்சியை தூண்டுவது எது? </t>
+  </si>
+  <si>
+    <t>எந்த நிகழ்வு தாவர வளர்ச்சியில் நடைபெறும் மூப்படைதல் எனும் நிகழ்ச்சியை தெரிவிக்கிறது?</t>
+  </si>
+  <si>
+    <t>ஓர் செயற்கையான வளர்ப்பு முறையில் வேறுபாடு அடையச் செய்வதற்கு,  உங்களிடம் திசு கொடுக்கப்படுகிறது. கீழ்க்கண்ட எந்த இரண்டு ஹார்மோன்களை வளர்ப்பு ஊடகத்தில் நீங்கள் சேர்ப்பதால், திசுவிலிருந்து வேர் மற்றும் தண்டுத்தொகுப்பு உருவாக்கப்படுகிறது?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">நேரான வடிவம் </t>
+  </si>
+  <si>
+    <t xml:space="preserve">பரவளைய வடிவம் </t>
+  </si>
+  <si>
+    <t>சிக்மாய்டு வடிவம்</t>
+  </si>
+  <si>
+    <t>பைட்டோகுரோம் என்பது என்ன?</t>
+  </si>
+  <si>
+    <t>தாவரங்களில் வளர்ச்சி வளைவின் வடிவம் என்ன?</t>
+  </si>
+  <si>
+    <t>அவினா வளைவுச் சோதனை எனும் உயிரியல் ஆய்வு எதனுடைய செயல்பாட்டினை அறிய உதவுகிறது?</t>
+  </si>
+  <si>
+    <t>கிரப்ஸ் சுழற்சியில் உள்ள எந்த 5-கார்பன் கரிமசேர்மம் N2 வளர்சிதை மாற்றத்தில் முக்கிய சேர்மமாக உள்ளது?</t>
+  </si>
+  <si>
+    <t>காற்று மற்றும் காற்றிலா சுவாசித்தலில் பொதுவான நிலை எனப்படுவது?</t>
   </si>
 </sst>
 </file>
@@ -2158,7 +2158,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="C16" t="s">
         <v>89</v>
@@ -2761,7 +2761,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="C37" t="s">
         <v>200</v>
@@ -2877,7 +2877,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>217</v>
+        <v>315</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
@@ -2886,16 +2886,16 @@
         <v>2016</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="H41" s="2" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="I41">
         <v>4</v>
@@ -2906,25 +2906,25 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C42" t="s">
         <v>221</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>222</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>223</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>224</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>225</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>226</v>
-      </c>
-      <c r="H42" t="s">
-        <v>227</v>
       </c>
       <c r="I42">
         <v>4</v>
@@ -2935,7 +2935,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="C43" t="s">
         <v>10</v>
@@ -2944,16 +2944,16 @@
         <v>2017</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="I43">
         <v>3</v>
@@ -2964,7 +2964,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="C44" t="s">
         <v>10</v>
@@ -2973,16 +2973,16 @@
         <v>2013</v>
       </c>
       <c r="E44" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="G44" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="H44" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="I44">
         <v>1</v>
@@ -2993,7 +2993,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C45" t="s">
         <v>140</v>
@@ -3002,16 +3002,16 @@
         <v>2010</v>
       </c>
       <c r="E45" t="s">
+        <v>229</v>
+      </c>
+      <c r="F45" t="s">
         <v>230</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>231</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>232</v>
-      </c>
-      <c r="H45" t="s">
-        <v>233</v>
       </c>
       <c r="I45">
         <v>2</v>
@@ -3022,54 +3022,54 @@
         <v>45</v>
       </c>
       <c r="B46" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C46" t="s">
         <v>234</v>
-      </c>
-      <c r="C46" t="s">
-        <v>235</v>
       </c>
       <c r="D46">
         <v>1980</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="H46" s="9" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
       <c r="I46" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>46</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>237</v>
+        <v>314</v>
       </c>
       <c r="C47" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D47">
         <v>1980</v>
       </c>
       <c r="E47" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="H47" s="9" t="s">
         <v>238</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>241</v>
       </c>
       <c r="I47" s="9">
         <v>3</v>
@@ -3080,25 +3080,25 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>242</v>
+        <v>333</v>
       </c>
       <c r="C48" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D48">
         <v>1984</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="H48" s="9" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I48" s="9">
         <v>1</v>
@@ -3109,7 +3109,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>247</v>
+        <v>316</v>
       </c>
       <c r="C49" t="s">
         <v>101</v>
@@ -3118,16 +3118,16 @@
         <v>1984</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="I49" s="9">
         <v>3</v>
@@ -3138,7 +3138,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>252</v>
+        <v>332</v>
       </c>
       <c r="C50" t="s">
         <v>101</v>
@@ -3147,16 +3147,16 @@
         <v>1989</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="H50" s="9" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="I50" s="9">
         <v>4</v>
@@ -3167,25 +3167,25 @@
         <v>50</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C51" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D51">
         <v>2000</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="H51" s="9" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="I51" s="9">
         <v>2</v>
@@ -3196,25 +3196,25 @@
         <v>51</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>263</v>
+        <v>317</v>
       </c>
       <c r="C52" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="D52">
         <v>2003</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="I52" s="9">
         <v>4</v>
@@ -3225,7 +3225,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>269</v>
+        <v>318</v>
       </c>
       <c r="C53" t="s">
         <v>45</v>
@@ -3234,16 +3234,16 @@
         <v>2004</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="I53" s="9">
         <v>1</v>
@@ -3254,7 +3254,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>273</v>
+        <v>319</v>
       </c>
       <c r="C54" t="s">
         <v>101</v>
@@ -3263,16 +3263,16 @@
         <v>2004</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="I54" s="9">
         <v>3</v>
@@ -3283,25 +3283,25 @@
         <v>54</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C55" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="D55" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="H55" s="9" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="I55" s="8">
         <v>1</v>
@@ -3312,7 +3312,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C56" t="s">
         <v>140</v>
@@ -3321,16 +3321,16 @@
         <v>2004</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="I56" s="9">
         <v>2</v>
@@ -3341,36 +3341,36 @@
         <v>56</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>281</v>
+        <v>321</v>
       </c>
       <c r="C57" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D57">
         <v>2009</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="H57" s="9" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="I57" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>57</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>287</v>
+        <v>322</v>
       </c>
       <c r="C58" t="s">
         <v>140</v>
@@ -3379,16 +3379,16 @@
         <v>2010</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="I58" s="9">
         <v>2</v>
@@ -3399,7 +3399,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="C59" t="s">
         <v>140</v>
@@ -3408,16 +3408,16 @@
         <v>2010</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="I59" s="9">
         <v>3</v>
@@ -3428,7 +3428,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>293</v>
+        <v>323</v>
       </c>
       <c r="C60" t="s">
         <v>140</v>
@@ -3437,16 +3437,16 @@
         <v>2010</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H60" s="9" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="I60" s="9">
         <v>1</v>
@@ -3457,7 +3457,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>295</v>
+        <v>324</v>
       </c>
       <c r="C61" t="s">
         <v>140</v>
@@ -3466,16 +3466,16 @@
         <v>2008</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="H61" s="9" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="I61" s="9">
         <v>4</v>
@@ -3486,7 +3486,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C62" t="s">
         <v>10</v>
@@ -3495,16 +3495,16 @@
         <v>2016</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="H62" s="9" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="I62" s="9">
         <v>3</v>
@@ -3515,7 +3515,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>304</v>
+        <v>329</v>
       </c>
       <c r="C63" t="s">
         <v>10</v>
@@ -3524,16 +3524,16 @@
         <v>2016</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="H63" s="8" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="I63" s="9">
         <v>1</v>
@@ -3544,7 +3544,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
       <c r="C64" t="s">
         <v>10</v>
@@ -3553,16 +3553,16 @@
         <v>2016</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>312</v>
+        <v>327</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
       <c r="I64" s="9">
         <v>4</v>

</xml_diff>

<commit_message>
fixing a sentennce - tamil semantically correct
</commit_message>
<xml_diff>
--- a/tamil_biology/unit_05_plant_physiology.xlsx
+++ b/tamil_biology/unit_05_plant_physiology.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2020\git\tvmani.github.io\tamil_biology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95306649-ED69-4954-B67A-AE1636897CA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F10B218-A452-4291-BC6A-E92143CB2BFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1219,9 +1219,6 @@
     <t>பைட்டோகுரோம் என்பது என்ன?</t>
   </si>
   <si>
-    <t>தாவரங்களில் வளர்ச்சி வளைவின் வடிவம் என்ன?</t>
-  </si>
-  <si>
     <t>அவினா வளைவுச் சோதனை எனும் உயிரியல் ஆய்வு எதனுடைய செயல்பாட்டினை அறிய உதவுகிறது?</t>
   </si>
   <si>
@@ -1229,6 +1226,9 @@
   </si>
   <si>
     <t>காற்று மற்றும் காற்றிலா சுவாசித்தலில் பொதுவான நிலை எனப்படுவது?</t>
+  </si>
+  <si>
+    <t>தாவரங்களில் வளர்ச்சி வளைவின் வடிவம் எப்படி இருக்கும்?</t>
   </si>
 </sst>
 </file>
@@ -1703,7 +1703,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3080,7 +3082,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C48" t="s">
         <v>234</v>
@@ -3138,7 +3140,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C50" t="s">
         <v>101</v>
@@ -3283,7 +3285,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C55" t="s">
         <v>267</v>
@@ -3544,7 +3546,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="C64" t="s">
         <v>10</v>

</xml_diff>